<commit_message>
all new variables added 1 YRs
</commit_message>
<xml_diff>
--- a/data guides/figureguide.xlsx
+++ b/data guides/figureguide.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmccall\Documents\GIT\Regional Planning\1. Comprehensive Plans\data guides\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmccall\Documents\GIT\Parent-Data-Gathering\data guides\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32655E05-0CAA-467C-B88F-FFF2A31B0043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5099F632-6EDA-4E3D-BADB-9B48331684C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="348" xr2:uid="{88FB4A29-507E-4A7F-AB27-0C12CA19CCD5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="348" xr2:uid="{88FB4A29-507E-4A7F-AB27-0C12CA19CCD5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="241">
   <si>
     <t>Figure Title</t>
   </si>
@@ -698,6 +698,66 @@
   </si>
   <si>
     <t>line showing number over time for available years 2020, 2025 if not weird, 2035, 2045</t>
+  </si>
+  <si>
+    <t>crash data funnel through me from Ashleigh</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>Means of Transportation to work</t>
+  </si>
+  <si>
+    <t>stacked bar for regular geographies all categories</t>
+  </si>
+  <si>
+    <t>trend line for only work from home last t10 years GOI</t>
+  </si>
+  <si>
+    <t>percent of commutes in GOI over 45 and 90 minutes all 3 years double bar - if 90 isn't significant then drop it or change to a diff category</t>
+  </si>
+  <si>
+    <t>vehicles avail</t>
+  </si>
+  <si>
+    <t>no vehicles, 1 vehicle, 2 or more, leave 3 years and leave county and state, or place county and state - don't need to know incorporated vs unincorporated</t>
+  </si>
+  <si>
+    <t>Public Health and Safety</t>
+  </si>
+  <si>
+    <t>food insecurity same figure type but regular group of geos</t>
+  </si>
+  <si>
+    <t>w and w/o health insurance figures same types but regular geographies - not incorporated vs unincorporated</t>
+  </si>
+  <si>
+    <t>h insurance by type good fig but regular geographies not incorporated vs unincorporated</t>
+  </si>
+  <si>
+    <t>county health rankings - do a gradient table with comparative counties, or just report the GOI</t>
+  </si>
+  <si>
+    <t>premature deaths - make something way simpler… add timeline if its available</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age adjusted death rate - just a percent for the GOI for 2010 and current if available </t>
+  </si>
+  <si>
+    <t>leading cause of death regular geographies maybe just top 3, replace the rates - add up all numbers and then find the percent of the total to say "50% of people dying in x county are dying from 1, 2, 3 at 20%, 20%, and 10%"</t>
+  </si>
+  <si>
+    <t>physical and mental distress leave as is - put axes on same scale, include a description</t>
+  </si>
+  <si>
+    <t>crime rate per thousand replace with regular geographies</t>
+  </si>
+  <si>
+    <t>same ^ with violent crime rate</t>
+  </si>
+  <si>
+    <t>for top arrests by type do one tree plot for GOI</t>
   </si>
 </sst>
 </file>
@@ -753,10 +813,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1083,10 +1142,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4107CF3D-677C-4E65-8005-86AF33A7710D}">
   <dimension ref="A1:K94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="H77" sqref="H77"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,7 +1198,7 @@
       <c r="B2" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
@@ -1171,7 +1230,7 @@
       <c r="B3" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>97</v>
       </c>
       <c r="D3" t="s">
@@ -1203,7 +1262,7 @@
       <c r="B4" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D4" t="s">
@@ -1232,7 +1291,7 @@
       <c r="B5" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
@@ -1258,13 +1317,13 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>218</v>
       </c>
       <c r="B6" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" t="s">
         <v>20</v>
       </c>
       <c r="D6" t="s">
@@ -1290,11 +1349,11 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
+      <c r="A7" s="4"/>
       <c r="B7" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" t="s">
         <v>22</v>
       </c>
       <c r="D7" t="s">
@@ -1320,11 +1379,11 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
+      <c r="A8" s="4"/>
       <c r="B8" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" t="s">
         <v>23</v>
       </c>
       <c r="D8" t="s">
@@ -1353,7 +1412,7 @@
       <c r="B9" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D9" t="s">
@@ -1382,7 +1441,7 @@
       <c r="B10" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D10" t="s">
@@ -1411,7 +1470,7 @@
       <c r="B11" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D11" t="s">
@@ -1440,7 +1499,7 @@
       <c r="B12" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D12" t="s">
@@ -1469,7 +1528,7 @@
       <c r="B13" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>128</v>
       </c>
       <c r="D13" t="s">
@@ -1498,7 +1557,7 @@
       <c r="B14" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>58</v>
       </c>
       <c r="D14" t="s">
@@ -1527,7 +1586,7 @@
       <c r="B15" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>53</v>
       </c>
       <c r="D15" t="s">
@@ -1556,7 +1615,7 @@
       <c r="B16" t="s">
         <v>64</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>54</v>
       </c>
       <c r="D16" t="s">
@@ -1585,7 +1644,7 @@
       <c r="B17" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D17" t="s">
@@ -1614,7 +1673,7 @@
       <c r="B18" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>56</v>
       </c>
       <c r="D18" t="s">
@@ -1643,7 +1702,7 @@
       <c r="B19" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>65</v>
       </c>
       <c r="D19" t="s">
@@ -1672,7 +1731,7 @@
       <c r="B20" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>125</v>
       </c>
       <c r="D20" t="s">
@@ -1701,7 +1760,7 @@
       <c r="B21" t="s">
         <v>65</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>124</v>
       </c>
       <c r="D21" t="s">
@@ -1730,7 +1789,7 @@
       <c r="B22" t="s">
         <v>65</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D22" t="s">
@@ -1759,7 +1818,7 @@
       <c r="B23" t="s">
         <v>65</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>69</v>
       </c>
       <c r="D23" t="s">
@@ -1788,7 +1847,7 @@
       <c r="B24" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D24" t="s">
@@ -1820,7 +1879,7 @@
       <c r="B25" t="s">
         <v>65</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D25" t="s">
@@ -1852,7 +1911,7 @@
       <c r="B26" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="3" t="s">
         <v>76</v>
       </c>
       <c r="D26" t="s">
@@ -1884,7 +1943,7 @@
       <c r="B27" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="3" t="s">
         <v>77</v>
       </c>
       <c r="D27" t="s">
@@ -1916,7 +1975,7 @@
       <c r="B28" t="s">
         <v>84</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>84</v>
       </c>
       <c r="D28" t="s">
@@ -1945,7 +2004,7 @@
       <c r="B29" t="s">
         <v>84</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>138</v>
       </c>
       <c r="E29">
@@ -1971,7 +2030,7 @@
       <c r="B30" t="s">
         <v>83</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>83</v>
       </c>
       <c r="D30" t="s">
@@ -2029,7 +2088,7 @@
       <c r="B32" t="s">
         <v>85</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>86</v>
       </c>
       <c r="D32" t="s">
@@ -2814,7 +2873,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="65" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
         <v>199</v>
       </c>
@@ -2834,7 +2893,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="66" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
         <v>200</v>
       </c>
@@ -2857,7 +2916,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="67" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
         <v>202</v>
       </c>
@@ -2874,7 +2933,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="68" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
         <v>204</v>
       </c>
@@ -2897,7 +2956,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="69" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D69" t="s">
         <v>36</v>
       </c>
@@ -2908,7 +2967,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="70" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D70" t="s">
         <v>36</v>
       </c>
@@ -2919,7 +2978,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="71" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D71" t="s">
         <v>36</v>
       </c>
@@ -2930,7 +2989,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="72" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
         <v>36</v>
       </c>
@@ -2941,7 +3000,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="73" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D73" t="s">
         <v>36</v>
       </c>
@@ -2952,7 +3011,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="74" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D74" t="s">
         <v>36</v>
       </c>
@@ -2966,7 +3025,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="75" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D75" t="s">
         <v>36</v>
       </c>
@@ -2977,7 +3036,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="76" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D76" t="s">
         <v>36</v>
       </c>
@@ -2988,7 +3047,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="77" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D77" t="s">
         <v>36</v>
       </c>
@@ -2999,7 +3058,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="78" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D78" t="s">
         <v>36</v>
       </c>
@@ -3010,132 +3069,195 @@
         <v>217</v>
       </c>
     </row>
-    <row r="79" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>222</v>
+      </c>
       <c r="D79" t="s">
         <v>36</v>
       </c>
       <c r="E79">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="H79" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>222</v>
+      </c>
+      <c r="C80" t="s">
+        <v>223</v>
+      </c>
       <c r="D80" t="s">
         <v>36</v>
       </c>
       <c r="E80">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="H80" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D81" t="s">
         <v>36</v>
       </c>
       <c r="E81">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="H81" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D82" t="s">
         <v>36</v>
       </c>
       <c r="E82">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="H82" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D83" t="s">
         <v>36</v>
       </c>
       <c r="E83">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="G83" t="s">
+        <v>227</v>
+      </c>
+      <c r="H83" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>229</v>
+      </c>
       <c r="D84" t="s">
         <v>36</v>
       </c>
       <c r="E84">
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="H84" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D85" t="s">
         <v>36</v>
       </c>
       <c r="E85">
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="H85" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D86" t="s">
         <v>36</v>
       </c>
       <c r="E86">
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="H86" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D87" t="s">
         <v>36</v>
       </c>
       <c r="E87">
         <v>86</v>
       </c>
-    </row>
-    <row r="88" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="H87" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D88" t="s">
         <v>36</v>
       </c>
       <c r="E88">
         <v>87</v>
       </c>
-    </row>
-    <row r="89" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="H88" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D89" t="s">
         <v>36</v>
       </c>
       <c r="E89">
         <v>88</v>
       </c>
-    </row>
-    <row r="90" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="H89" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D90" t="s">
         <v>36</v>
       </c>
       <c r="E90">
         <v>89</v>
       </c>
-    </row>
-    <row r="91" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="H90" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D91" t="s">
         <v>36</v>
       </c>
       <c r="E91">
         <v>90</v>
       </c>
-    </row>
-    <row r="92" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="H91" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D92" t="s">
         <v>36</v>
       </c>
       <c r="E92">
         <v>91</v>
       </c>
-    </row>
-    <row r="93" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="H92" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D93" t="s">
         <v>36</v>
       </c>
       <c r="E93">
         <v>92</v>
       </c>
-    </row>
-    <row r="94" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="H93" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D94" t="s">
         <v>36</v>
       </c>
       <c r="E94">
         <v>93</v>
+      </c>
+      <c r="H94" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>